<commit_message>
Update for Week 11
</commit_message>
<xml_diff>
--- a/weather_2025_raw.xlsx
+++ b/weather_2025_raw.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\football_stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2974A3CC-DF6B-41E2-AEEA-C4F3E1C83FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211986DF-A9F4-44FE-ACF6-E06B73BC9DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Week 10" sheetId="8" r:id="rId1"/>
-    <sheet name="Week 9" sheetId="7" r:id="rId2"/>
-    <sheet name="Week 8" sheetId="6" r:id="rId3"/>
-    <sheet name="Week 7" sheetId="5" r:id="rId4"/>
-    <sheet name="Week 6" sheetId="4" r:id="rId5"/>
-    <sheet name="Week 5" sheetId="3" r:id="rId6"/>
-    <sheet name="Week 4" sheetId="2" r:id="rId7"/>
-    <sheet name="Week 3" sheetId="1" r:id="rId8"/>
+    <sheet name="Week 11" sheetId="9" r:id="rId1"/>
+    <sheet name="Week 10" sheetId="8" r:id="rId2"/>
+    <sheet name="Week 9" sheetId="7" r:id="rId3"/>
+    <sheet name="Week 8" sheetId="6" r:id="rId4"/>
+    <sheet name="Week 7" sheetId="5" r:id="rId5"/>
+    <sheet name="Week 6" sheetId="4" r:id="rId6"/>
+    <sheet name="Week 5" sheetId="3" r:id="rId7"/>
+    <sheet name="Week 4" sheetId="2" r:id="rId8"/>
+    <sheet name="Week 3" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
   <si>
     <t>game</t>
   </si>
@@ -385,6 +386,39 @@
   </si>
   <si>
     <t>GBvsPHI</t>
+  </si>
+  <si>
+    <t>NEvsNYJ</t>
+  </si>
+  <si>
+    <t>MIAvsWAS</t>
+  </si>
+  <si>
+    <t>BUFvsTB</t>
+  </si>
+  <si>
+    <t>CHIvsMIN</t>
+  </si>
+  <si>
+    <t>GBvsNYG</t>
+  </si>
+  <si>
+    <t>JAXvsLAC</t>
+  </si>
+  <si>
+    <t>LAvsSEA</t>
+  </si>
+  <si>
+    <t>BALvsCLE</t>
+  </si>
+  <si>
+    <t>DENvsKC</t>
+  </si>
+  <si>
+    <t>DETvsPHI</t>
+  </si>
+  <si>
+    <t>DALvsLV</t>
   </si>
 </sst>
 </file>
@@ -755,8 +789,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E5F55B-DA42-4A8B-8113-C12FFA893649}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640C47C7-0E74-493C-8539-6011056153AB}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -777,87 +811,87 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B8">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="B9">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -865,68 +899,79 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="B10">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16">
+        <v>56</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -935,6 +980,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E5F55B-DA42-4A8B-8113-C12FFA893649}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2">
+        <v>54</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>81</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>57</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E6C2C3-BC8C-4DD8-B0A7-8E3DE38351AD}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -1114,7 +1339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C632E301-E10A-4468-8562-2A2AA9DD2201}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -1283,7 +1508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4232272C-E69B-4889-80D9-17C7620F0DD5}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -1474,7 +1699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117E9C0E-235D-4A2C-9655-79A7010A5632}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -1665,7 +1890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5819D80-3B90-4A7B-938D-5D525A7FC316}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -1845,7 +2070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A046177-1C33-461B-A466-912B82D45403}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -2047,7 +2272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3048DBF6-8581-4081-B5BC-5366E09C39A7}">
   <dimension ref="A1:C17"/>
   <sheetViews>

</xml_diff>